<commit_message>
Dud multiplieer for NanoMol-PER-MicroGM-HR fixed
</commit_message>
<xml_diff>
--- a/community/NVS-P06/P06-additions-to-QUDT.xlsx
+++ b/community/NVS-P06/P06-additions-to-QUDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cox075\dev\qudt-public-repo\community\NVS-P06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A403FC-1EBD-49ED-B8CD-9B5FE6790FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082761A7-E7D1-4EF9-AF12-C2DEBC95BED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="3720" windowWidth="31815" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="4305" windowWidth="36225" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qudt-requests" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="695">
   <si>
     <t xml:space="preserve"> unit:BQ-SEC-PER-M3</t>
   </si>
@@ -1007,9 +1007,6 @@
   </si>
   <si>
     <t xml:space="preserve">W.s.m-2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mol.kg-1.s-1 </t>
   </si>
   <si>
     <t>Becquerels second per cubic metre</t>
@@ -3111,15 +3108,18 @@
   <dimension ref="A1:N186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="14" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I131" sqref="I131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="6" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="29.7109375" customWidth="1"/>
@@ -3128,10 +3128,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G1" s="5"/>
       <c r="I1" s="5"/>
@@ -3140,13 +3140,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>579</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>580</v>
       </c>
       <c r="G2" s="5"/>
       <c r="I2" s="5"/>
@@ -3154,13 +3154,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="5"/>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G4" s="5"/>
       <c r="I4" s="5"/>
@@ -3186,13 +3186,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>581</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>582</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="5"/>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>567</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>568</v>
       </c>
       <c r="G6" s="5"/>
       <c r="I6" s="5"/>
@@ -3216,13 +3216,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>566</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G7" s="5"/>
       <c r="I7" s="5"/>
@@ -3232,13 +3232,13 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G8" s="5"/>
       <c r="I8" s="5"/>
@@ -3248,13 +3248,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>593</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>594</v>
       </c>
       <c r="G9" s="5"/>
       <c r="I9" s="5"/>
@@ -3264,10 +3264,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C13" s="5"/>
       <c r="G13" s="5"/>
@@ -3311,34 +3311,34 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>572</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>573</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>574</v>
-      </c>
       <c r="D14" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F14" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>590</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>596</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>595</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>592</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>591</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="12"/>
@@ -3346,20 +3346,20 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B15" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C15" t="s">
+        <v>551</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>553</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J15" t="s">
         <v>308</v>
@@ -3370,19 +3370,19 @@
         <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C16" t="s">
+        <v>461</v>
+      </c>
+      <c r="D16" t="s">
         <v>462</v>
       </c>
-      <c r="D16" t="s">
-        <v>463</v>
-      </c>
       <c r="E16" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F16" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I16">
         <v>1000</v>
@@ -3396,19 +3396,19 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C17" t="s">
+        <v>329</v>
+      </c>
+      <c r="D17" t="s">
         <v>330</v>
       </c>
-      <c r="D17" t="s">
-        <v>331</v>
-      </c>
       <c r="E17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -3422,16 +3422,16 @@
         <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F18" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I18">
         <v>100</v>
@@ -3442,28 +3442,28 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>560</v>
+      </c>
+      <c r="B19" t="s">
+        <v>588</v>
+      </c>
+      <c r="C19" t="s">
         <v>561</v>
       </c>
-      <c r="B19" t="s">
-        <v>589</v>
-      </c>
-      <c r="C19" t="s">
-        <v>562</v>
-      </c>
       <c r="D19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F19" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I19">
         <v>1E-4</v>
       </c>
       <c r="J19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3471,19 +3471,19 @@
         <v>185</v>
       </c>
       <c r="B20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F20" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I20" s="1">
         <v>3.1688087814028902E-13</v>
@@ -3497,19 +3497,19 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C21" t="s">
+        <v>331</v>
+      </c>
+      <c r="D21" t="s">
         <v>332</v>
       </c>
-      <c r="D21" t="s">
-        <v>333</v>
-      </c>
       <c r="E21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I21" s="1">
         <v>1.0000000000000001E-18</v>
@@ -3520,19 +3520,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C22" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F22" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -3546,16 +3546,16 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C23" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" t="s">
         <v>338</v>
       </c>
-      <c r="D23" t="s">
-        <v>339</v>
-      </c>
       <c r="F23" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -3569,16 +3569,16 @@
         <v>267</v>
       </c>
       <c r="B24" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F24" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -3592,19 +3592,19 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C25" t="s">
+        <v>333</v>
+      </c>
+      <c r="D25" t="s">
         <v>334</v>
       </c>
-      <c r="D25" t="s">
-        <v>335</v>
-      </c>
       <c r="E25" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F25" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -3618,16 +3618,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D26" t="s">
         <v>336</v>
       </c>
-      <c r="D26" t="s">
-        <v>337</v>
-      </c>
       <c r="F26" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -3641,25 +3641,25 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C27" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" t="s">
         <v>342</v>
       </c>
-      <c r="D27" t="s">
-        <v>343</v>
-      </c>
       <c r="E27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F27" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G27" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H27" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I27" s="1">
         <v>1.0000000000000001E-18</v>
@@ -3673,19 +3673,19 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D28" t="s">
         <v>344</v>
       </c>
-      <c r="D28" t="s">
-        <v>345</v>
-      </c>
       <c r="E28" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I28" s="1">
         <v>1.0000000000000001E-15</v>
@@ -3699,19 +3699,19 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C29" t="s">
+        <v>345</v>
+      </c>
+      <c r="D29" t="s">
         <v>346</v>
       </c>
-      <c r="D29" t="s">
-        <v>347</v>
-      </c>
       <c r="E29" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F29" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I29" s="1">
         <v>1.0000000000000001E-15</v>
@@ -3725,19 +3725,19 @@
         <v>275</v>
       </c>
       <c r="B30" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C30" t="s">
+        <v>517</v>
+      </c>
+      <c r="D30" t="s">
         <v>518</v>
       </c>
-      <c r="D30" t="s">
-        <v>519</v>
-      </c>
       <c r="E30" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I30" s="1">
         <v>9.9999999999999998E-13</v>
@@ -3751,16 +3751,16 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C31" t="s">
+        <v>347</v>
+      </c>
+      <c r="D31" t="s">
         <v>348</v>
       </c>
-      <c r="D31" t="s">
-        <v>349</v>
-      </c>
       <c r="F31" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I31" s="1">
         <v>3.1688087814028901E-7</v>
@@ -3774,19 +3774,19 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C32" t="s">
+        <v>349</v>
+      </c>
+      <c r="D32" t="s">
         <v>350</v>
       </c>
-      <c r="D32" t="s">
-        <v>351</v>
-      </c>
       <c r="E32" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F32" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I32">
         <v>2.7777777777777801E-2</v>
@@ -3800,19 +3800,19 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C33" t="s">
+        <v>351</v>
+      </c>
+      <c r="D33" t="s">
         <v>352</v>
       </c>
-      <c r="D33" t="s">
-        <v>353</v>
-      </c>
       <c r="E33" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F33" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I33">
         <v>0.115740740740741</v>
@@ -3826,16 +3826,16 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C34" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F34" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -3849,16 +3849,16 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F35" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -3872,16 +3872,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F36" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -3895,19 +3895,19 @@
         <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C37" t="s">
+        <v>355</v>
+      </c>
+      <c r="D37" t="s">
         <v>356</v>
       </c>
-      <c r="D37" t="s">
-        <v>357</v>
-      </c>
       <c r="E37" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F37" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I37">
         <v>9.9999999999999995E-7</v>
@@ -3921,19 +3921,19 @@
         <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C38" t="s">
+        <v>357</v>
+      </c>
+      <c r="D38" t="s">
         <v>358</v>
       </c>
-      <c r="D38" t="s">
-        <v>359</v>
-      </c>
       <c r="E38" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F38" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I38">
         <v>2.7777777777777799E-4</v>
@@ -3947,19 +3947,19 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C39" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D39" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E39" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F39" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -3973,19 +3973,19 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C40" t="s">
+        <v>364</v>
+      </c>
+      <c r="D40" t="s">
         <v>365</v>
       </c>
-      <c r="D40" t="s">
-        <v>366</v>
-      </c>
       <c r="E40" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F40" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I40">
         <v>1.1574074074074099E-2</v>
@@ -3999,19 +3999,19 @@
         <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C41" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E41" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F41" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -4025,16 +4025,16 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C42" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F42" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -4048,16 +4048,16 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F43" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -4071,16 +4071,16 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F44" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -4094,16 +4094,16 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C45" t="s">
+        <v>339</v>
+      </c>
+      <c r="D45" t="s">
         <v>340</v>
       </c>
-      <c r="D45" t="s">
-        <v>341</v>
-      </c>
       <c r="F45" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -4117,16 +4117,16 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C46" t="s">
+        <v>371</v>
+      </c>
+      <c r="D46" t="s">
         <v>372</v>
       </c>
-      <c r="D46" t="s">
-        <v>373</v>
-      </c>
       <c r="F46" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -4137,22 +4137,22 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B47" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C47" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E47" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F47" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -4163,19 +4163,19 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B48" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F48" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -4189,19 +4189,19 @@
         <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C49" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E49" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F49" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -4215,19 +4215,19 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C50" t="s">
+        <v>376</v>
+      </c>
+      <c r="D50" t="s">
         <v>377</v>
       </c>
-      <c r="D50" t="s">
-        <v>378</v>
-      </c>
       <c r="E50" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F50" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I50">
         <v>1000</v>
@@ -4241,19 +4241,19 @@
         <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C51" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D51" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F51" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I51">
         <v>1</v>
@@ -4267,16 +4267,16 @@
         <v>237</v>
       </c>
       <c r="B52" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C52" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D52" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F52" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I52">
         <v>1</v>
@@ -4290,16 +4290,16 @@
         <v>239</v>
       </c>
       <c r="B53" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C53" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D53" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F53" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -4313,16 +4313,16 @@
         <v>241</v>
       </c>
       <c r="B54" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C54" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F54" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -4333,22 +4333,22 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B55" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C55" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D55" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E55" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F55" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I55">
         <v>1000</v>
@@ -4359,22 +4359,22 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>549</v>
+      </c>
+      <c r="B56" t="s">
+        <v>588</v>
+      </c>
+      <c r="C56" t="s">
         <v>550</v>
       </c>
-      <c r="B56" t="s">
-        <v>589</v>
-      </c>
-      <c r="C56" t="s">
-        <v>551</v>
-      </c>
       <c r="D56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E56" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F56" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I56">
         <v>1000</v>
@@ -4388,16 +4388,16 @@
         <v>222</v>
       </c>
       <c r="B57" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C57" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F57" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -4411,16 +4411,16 @@
         <v>243</v>
       </c>
       <c r="B58" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C58" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F58" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -4434,16 +4434,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C59" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D59" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F59" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I59">
         <v>57.295779513082302</v>
@@ -4454,25 +4454,25 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>557</v>
+      </c>
+      <c r="B60" t="s">
+        <v>588</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="B60" t="s">
-        <v>589</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>559</v>
-      </c>
       <c r="D60" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F60" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I60">
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -4480,16 +4480,16 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C61" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D61" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F61" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I61">
         <v>1</v>
@@ -4503,16 +4503,16 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D62" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F62" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -4526,19 +4526,19 @@
         <v>179</v>
       </c>
       <c r="B63" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C63" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D63" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E63" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I63">
         <v>0.101325</v>
@@ -4552,19 +4552,19 @@
         <v>313</v>
       </c>
       <c r="B64" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C64" t="s">
+        <v>537</v>
+      </c>
+      <c r="D64" t="s">
         <v>538</v>
       </c>
-      <c r="D64" t="s">
-        <v>539</v>
-      </c>
       <c r="E64" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F64" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I64">
         <v>9.9999999999999995E-7</v>
@@ -4578,19 +4578,19 @@
         <v>304</v>
       </c>
       <c r="B65" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C65" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D65" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E65" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F65" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I65">
         <v>1E-3</v>
@@ -4604,16 +4604,16 @@
         <v>210</v>
       </c>
       <c r="B66" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C66" t="s">
+        <v>479</v>
+      </c>
+      <c r="D66" t="s">
         <v>480</v>
       </c>
-      <c r="D66" t="s">
-        <v>481</v>
-      </c>
       <c r="F66" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I66" s="1">
         <v>1E-8</v>
@@ -4627,25 +4627,25 @@
         <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C67" t="s">
+        <v>473</v>
+      </c>
+      <c r="D67" t="s">
         <v>474</v>
       </c>
-      <c r="D67" t="s">
-        <v>475</v>
-      </c>
       <c r="E67" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F67" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G67" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H67" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I67">
         <v>9.9999999999999995E-7</v>
@@ -4659,16 +4659,16 @@
         <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C68" t="s">
+        <v>396</v>
+      </c>
+      <c r="D68" t="s">
         <v>397</v>
       </c>
-      <c r="D68" t="s">
-        <v>398</v>
-      </c>
       <c r="F68" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I68" s="1">
         <v>2.7777777777777802E-10</v>
@@ -4682,16 +4682,16 @@
         <v>306</v>
       </c>
       <c r="B69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C69" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D69" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F69" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I69" s="1">
         <v>1.1574074074074101E-14</v>
@@ -4705,16 +4705,16 @@
         <v>206</v>
       </c>
       <c r="B70" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D70" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F70" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I70" s="1">
         <v>2.77777777777778E-13</v>
@@ -4728,19 +4728,19 @@
         <v>216</v>
       </c>
       <c r="B71" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C71" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E71" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F71" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I71" s="1">
         <v>1.0000000000000001E-18</v>
@@ -4754,25 +4754,25 @@
         <v>183</v>
       </c>
       <c r="B72" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D72" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E72" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F72" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G72" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H72" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I72" s="1">
         <v>1.0000000000000001E-18</v>
@@ -4786,25 +4786,25 @@
         <v>196</v>
       </c>
       <c r="B73" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D73" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E73" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F73" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G73" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H73" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I73" s="1">
         <v>9.9999999999999998E-13</v>
@@ -4818,19 +4818,19 @@
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C74" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D74" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E74" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F74" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I74" s="1">
         <v>9.9999999999999995E-7</v>
@@ -4844,19 +4844,19 @@
         <v>291</v>
       </c>
       <c r="B75" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C75" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D75" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E75" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F75" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I75">
         <v>1E-3</v>
@@ -4870,16 +4870,16 @@
         <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C76" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D76" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F76" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I76" s="1">
         <v>2.7777777777777802E-7</v>
@@ -4893,16 +4893,16 @@
         <v>309</v>
       </c>
       <c r="B77" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C77" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D77" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F77" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I77" s="1">
         <v>1.1574074074074099E-11</v>
@@ -4916,16 +4916,16 @@
         <v>220</v>
       </c>
       <c r="B78" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C78" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D78" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F78" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I78" s="1">
         <v>2.7777777777777802E-10</v>
@@ -4939,16 +4939,16 @@
         <v>212</v>
       </c>
       <c r="B79" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C79" t="s">
+        <v>481</v>
+      </c>
+      <c r="D79" t="s">
         <v>482</v>
       </c>
-      <c r="D79" t="s">
-        <v>483</v>
-      </c>
       <c r="F79" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I79">
         <v>9.9999999999999995E-7</v>
@@ -4962,16 +4962,16 @@
         <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C80" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F80" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I80">
         <v>1.1574074074074101E-5</v>
@@ -4985,22 +4985,22 @@
         <v>232</v>
       </c>
       <c r="B81" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C81" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D81" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F81" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G81" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H81" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I81">
         <v>9.9999999999999995E-7</v>
@@ -5014,16 +5014,16 @@
         <v>224</v>
       </c>
       <c r="B82" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C82" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D82" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F82" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I82" s="1">
         <v>1.15740740740741E-8</v>
@@ -5037,16 +5037,16 @@
         <v>301</v>
       </c>
       <c r="B83" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C83" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D83" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F83" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I83">
         <v>9.9999999999999995E-7</v>
@@ -5060,19 +5060,19 @@
         <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C84" t="s">
+        <v>388</v>
+      </c>
+      <c r="D84" t="s">
         <v>389</v>
       </c>
-      <c r="D84" t="s">
-        <v>390</v>
-      </c>
       <c r="E84" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I84">
         <v>1</v>
@@ -5086,19 +5086,19 @@
         <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C85" t="s">
+        <v>392</v>
+      </c>
+      <c r="D85" t="s">
         <v>393</v>
       </c>
-      <c r="D85" t="s">
-        <v>394</v>
-      </c>
       <c r="E85" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F85" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I85">
         <v>1E-3</v>
@@ -5112,19 +5112,19 @@
         <v>214</v>
       </c>
       <c r="B86" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C86" t="s">
+        <v>483</v>
+      </c>
+      <c r="D86" t="s">
         <v>484</v>
       </c>
-      <c r="D86" t="s">
-        <v>485</v>
-      </c>
       <c r="E86" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F86" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I86" s="1">
         <v>1</v>
@@ -5138,16 +5138,16 @@
         <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C87" t="s">
+        <v>390</v>
+      </c>
+      <c r="D87" t="s">
         <v>391</v>
       </c>
-      <c r="D87" t="s">
-        <v>392</v>
-      </c>
       <c r="F87" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I87" s="1">
         <v>1.15740740740741E-8</v>
@@ -5161,16 +5161,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C88" t="s">
+        <v>398</v>
+      </c>
+      <c r="D88" t="s">
         <v>399</v>
       </c>
-      <c r="D88" t="s">
-        <v>400</v>
-      </c>
       <c r="F88" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I88" s="1">
         <v>3.8025705376834699E-10</v>
@@ -5184,19 +5184,19 @@
         <v>200</v>
       </c>
       <c r="B89" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C89" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D89" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E89" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F89" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I89" s="1">
         <v>1.1574074074074099E-11</v>
@@ -5210,19 +5210,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C90" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D90" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E90" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F90" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I90" s="1">
         <v>2.7777777777777802E-10</v>
@@ -5236,16 +5236,16 @@
         <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C91" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F91" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I91" s="1">
         <v>1.1574074074074099E-11</v>
@@ -5259,16 +5259,16 @@
         <v>204</v>
       </c>
       <c r="B92" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C92" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D92" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F92" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I92" s="1">
         <v>2.7777777777777802E-10</v>
@@ -5282,16 +5282,16 @@
         <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C93" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D93" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F93" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I93" s="1">
         <v>1.1574074074074099E-11</v>
@@ -5305,16 +5305,16 @@
         <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C94" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D94" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F94" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I94">
         <v>1E-3</v>
@@ -5328,16 +5328,16 @@
         <v>218</v>
       </c>
       <c r="B95" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C95" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D95" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F95" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I95" s="1">
         <v>1.15740740740741E-8</v>
@@ -5351,19 +5351,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C96" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D96" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E96" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F96" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I96">
         <v>1E-3</v>
@@ -5377,16 +5377,16 @@
         <v>82</v>
       </c>
       <c r="B97" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C97" t="s">
+        <v>394</v>
+      </c>
+      <c r="D97" t="s">
         <v>395</v>
       </c>
-      <c r="D97" t="s">
-        <v>396</v>
-      </c>
       <c r="F97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I97" s="1">
         <v>1.15740740740741E-8</v>
@@ -5400,22 +5400,22 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C98" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D98" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F98" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G98" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H98" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I98">
         <v>1E-3</v>
@@ -5429,16 +5429,16 @@
         <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C99" t="s">
+        <v>413</v>
+      </c>
+      <c r="D99" t="s">
         <v>414</v>
       </c>
-      <c r="D99" t="s">
-        <v>415</v>
-      </c>
       <c r="F99" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I99" s="1">
         <v>2.7777777777777802E-7</v>
@@ -5452,19 +5452,19 @@
         <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C100" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D100" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E100" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F100" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I100">
         <v>1E-3</v>
@@ -5478,16 +5478,16 @@
         <v>116</v>
       </c>
       <c r="B101" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C101" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D101" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F101" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I101">
         <v>10000000</v>
@@ -5501,16 +5501,16 @@
         <v>112</v>
       </c>
       <c r="B102" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C102" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F102" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I102">
         <v>1000000</v>
@@ -5524,16 +5524,16 @@
         <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C103" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D103" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F103" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I103">
         <v>1000000</v>
@@ -5547,16 +5547,16 @@
         <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C104" t="s">
+        <v>408</v>
+      </c>
+      <c r="D104" t="s">
         <v>409</v>
       </c>
-      <c r="D104" t="s">
-        <v>410</v>
-      </c>
       <c r="F104" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I104">
         <v>0.27777777777777801</v>
@@ -5570,16 +5570,16 @@
         <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C105" t="s">
+        <v>401</v>
+      </c>
+      <c r="D105" t="s">
         <v>402</v>
       </c>
-      <c r="D105" t="s">
-        <v>403</v>
-      </c>
       <c r="F105" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I105">
         <v>1</v>
@@ -5593,16 +5593,16 @@
         <v>62</v>
       </c>
       <c r="B106" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C106" t="s">
+        <v>380</v>
+      </c>
+      <c r="D106" t="s">
         <v>381</v>
       </c>
-      <c r="D106" t="s">
-        <v>382</v>
-      </c>
       <c r="F106" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I106">
         <v>1</v>
@@ -5616,16 +5616,16 @@
         <v>60</v>
       </c>
       <c r="B107" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C107" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D107" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F107" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I107">
         <v>1</v>
@@ -5639,16 +5639,16 @@
         <v>68</v>
       </c>
       <c r="B108" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C108" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D108" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F108" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I108">
         <v>1</v>
@@ -5662,16 +5662,16 @@
         <v>72</v>
       </c>
       <c r="B109" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C109" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D109" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F109" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I109">
         <v>1</v>
@@ -5685,16 +5685,16 @@
         <v>92</v>
       </c>
       <c r="B110" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C110" t="s">
+        <v>403</v>
+      </c>
+      <c r="D110" t="s">
         <v>404</v>
       </c>
-      <c r="D110" t="s">
-        <v>405</v>
-      </c>
       <c r="F110" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I110">
         <v>1</v>
@@ -5708,22 +5708,22 @@
         <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C111" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D111" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F111" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G111" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H111" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I111">
         <v>1</v>
@@ -5737,19 +5737,19 @@
         <v>104</v>
       </c>
       <c r="B112" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C112" t="s">
+        <v>411</v>
+      </c>
+      <c r="D112" t="s">
         <v>412</v>
       </c>
-      <c r="D112" t="s">
-        <v>413</v>
-      </c>
       <c r="E112" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F112" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I112" s="1">
         <v>3.1688087814028901E-8</v>
@@ -5763,19 +5763,19 @@
         <v>247</v>
       </c>
       <c r="B113" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C113" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E113" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F113" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I113">
         <v>9.9999999999999995E-7</v>
@@ -5789,19 +5789,19 @@
         <v>261</v>
       </c>
       <c r="B114" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C114" t="s">
+        <v>508</v>
+      </c>
+      <c r="D114" t="s">
         <v>509</v>
       </c>
-      <c r="D114" t="s">
-        <v>510</v>
-      </c>
       <c r="E114" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F114" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I114" s="1">
         <v>9.9999999999999998E-13</v>
@@ -5815,19 +5815,19 @@
         <v>253</v>
       </c>
       <c r="B115" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C115" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D115" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E115" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F115" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I115" s="1">
         <v>1.15740740740741E-17</v>
@@ -5841,19 +5841,19 @@
         <v>251</v>
       </c>
       <c r="B116" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C116" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D116" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E116" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F116" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I116" s="1">
         <v>1.0000000000000001E-9</v>
@@ -5867,19 +5867,19 @@
         <v>263</v>
       </c>
       <c r="B117" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C117" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D117" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E117" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F117" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I117">
         <v>1E-3</v>
@@ -5893,16 +5893,16 @@
         <v>126</v>
       </c>
       <c r="B118" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C118" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F118" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I118" s="1">
         <v>2.7777777777777802E-7</v>
@@ -5916,19 +5916,19 @@
         <v>30</v>
       </c>
       <c r="B119" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C119" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D119" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E119" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F119" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I119" s="1">
         <v>1.0000000000000001E-9</v>
@@ -5942,16 +5942,16 @@
         <v>255</v>
       </c>
       <c r="B120" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C120" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D120" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F120" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I120" s="1">
         <v>1.1574074074074099E-11</v>
@@ -5965,16 +5965,16 @@
         <v>257</v>
       </c>
       <c r="B121" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C121" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D121" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F121" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I121" s="1">
         <v>2.7777777777777802E-10</v>
@@ -5988,16 +5988,16 @@
         <v>140</v>
       </c>
       <c r="B122" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C122" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D122" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F122" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I122" s="1">
         <v>1.1574074074074101E-14</v>
@@ -6011,19 +6011,19 @@
         <v>128</v>
       </c>
       <c r="B123" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C123" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D123" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F123" t="s">
-        <v>677</v>
-      </c>
-      <c r="I123" t="s">
-        <v>329</v>
+        <v>676</v>
+      </c>
+      <c r="I123">
+        <v>2.7777777777777799E-4</v>
       </c>
       <c r="J123" t="s">
         <v>129</v>
@@ -6034,22 +6034,22 @@
         <v>132</v>
       </c>
       <c r="B124" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C124" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D124" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F124" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G124" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="H124" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I124">
         <v>1E-3</v>
@@ -6063,16 +6063,16 @@
         <v>130</v>
       </c>
       <c r="B125" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C125" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D125" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F125" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I125" s="1">
         <v>1.15740740740741E-8</v>
@@ -6086,16 +6086,16 @@
         <v>122</v>
       </c>
       <c r="B126" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C126" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D126" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F126" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I126">
         <v>1</v>
@@ -6109,16 +6109,16 @@
         <v>311</v>
       </c>
       <c r="B127" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C127" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D127" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F127" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I127" s="1">
         <v>3.1688087814028901E-7</v>
@@ -6132,16 +6132,16 @@
         <v>259</v>
       </c>
       <c r="B128" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C128" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D128" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F128" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I128">
         <v>1000</v>
@@ -6155,19 +6155,19 @@
         <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C129" t="s">
+        <v>425</v>
+      </c>
+      <c r="D129" t="s">
         <v>426</v>
       </c>
-      <c r="D129" t="s">
-        <v>427</v>
-      </c>
       <c r="E129" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F129" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I129">
         <v>1000000</v>
@@ -6181,16 +6181,16 @@
         <v>118</v>
       </c>
       <c r="B130" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C130" t="s">
+        <v>420</v>
+      </c>
+      <c r="D130" t="s">
         <v>421</v>
       </c>
-      <c r="D130" t="s">
-        <v>422</v>
-      </c>
       <c r="F130" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I130">
         <v>10</v>
@@ -6204,19 +6204,19 @@
         <v>134</v>
       </c>
       <c r="B131" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C131" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D131" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E131" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F131" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I131">
         <v>2.7777777777777799E-4</v>
@@ -6230,19 +6230,19 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C132" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D132" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E132" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F132" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I132">
         <v>2.7777777777777799E-4</v>
@@ -6256,19 +6256,19 @@
         <v>138</v>
       </c>
       <c r="B133" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C133" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D133" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E133" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F133" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I133">
         <v>9.9999999999999995E-7</v>
@@ -6282,19 +6282,19 @@
         <v>189</v>
       </c>
       <c r="B134" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C134" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D134" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E134" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F134" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I134">
         <v>1000</v>
@@ -6308,16 +6308,16 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C135" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D135" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F135" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I135">
         <v>1</v>
@@ -6331,19 +6331,19 @@
         <v>287</v>
       </c>
       <c r="B136" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C136" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D136" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E136" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F136" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I136">
         <v>1</v>
@@ -6357,19 +6357,19 @@
         <v>249</v>
       </c>
       <c r="B137" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C137" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D137" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E137" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F137" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I137">
         <v>1.1574074074074101E-5</v>
@@ -6383,19 +6383,19 @@
         <v>285</v>
       </c>
       <c r="B138" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C138" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D138" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E138" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F138" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I138">
         <v>1</v>
@@ -6409,19 +6409,19 @@
         <v>194</v>
       </c>
       <c r="B139" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C139" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D139" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E139" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F139" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I139">
         <v>1000000000</v>
@@ -6435,16 +6435,16 @@
         <v>120</v>
       </c>
       <c r="B140" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C140" t="s">
+        <v>422</v>
+      </c>
+      <c r="D140" t="s">
         <v>423</v>
       </c>
-      <c r="D140" t="s">
-        <v>424</v>
-      </c>
       <c r="F140" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I140">
         <v>1000000</v>
@@ -6458,19 +6458,19 @@
         <v>187</v>
       </c>
       <c r="B141" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C141" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D141" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E141" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F141" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I141">
         <v>1000000000000</v>
@@ -6484,19 +6484,19 @@
         <v>191</v>
       </c>
       <c r="B142" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C142" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D142" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E142" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F142" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I142">
         <v>1</v>
@@ -6510,16 +6510,16 @@
         <v>166</v>
       </c>
       <c r="B143" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C143" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D143" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F143" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I143">
         <v>1</v>
@@ -6533,16 +6533,16 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C144" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D144" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F144" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I144">
         <v>1</v>
@@ -6556,16 +6556,16 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C145" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D145" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F145" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I145">
         <v>1</v>
@@ -6579,16 +6579,16 @@
         <v>142</v>
       </c>
       <c r="B146" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C146" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D146" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F146" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I146">
         <v>1</v>
@@ -6602,19 +6602,19 @@
         <v>269</v>
       </c>
       <c r="B147" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C147" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D147" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E147" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F147" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I147">
         <v>1.1574074074074101E-5</v>
@@ -6628,19 +6628,19 @@
         <v>271</v>
       </c>
       <c r="B148" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C148" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D148" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E148" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F148" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I148">
         <v>2.7777777777777799E-4</v>
@@ -6654,16 +6654,16 @@
         <v>289</v>
       </c>
       <c r="B149" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C149" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D149" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F149" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I149">
         <v>1</v>
@@ -6677,19 +6677,19 @@
         <v>273</v>
       </c>
       <c r="B150" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C150" t="s">
+        <v>515</v>
+      </c>
+      <c r="D150" t="s">
         <v>516</v>
       </c>
-      <c r="D150" t="s">
-        <v>517</v>
-      </c>
       <c r="E150" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F150" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I150">
         <v>1.6534391534391499E-6</v>
@@ -6703,16 +6703,16 @@
         <v>148</v>
       </c>
       <c r="B151" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C151" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D151" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F151" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I151">
         <v>1000</v>
@@ -6726,19 +6726,19 @@
         <v>66</v>
       </c>
       <c r="B152" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C152" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D152" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E152" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F152" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I152">
         <v>1</v>
@@ -6752,16 +6752,16 @@
         <v>70</v>
       </c>
       <c r="B153" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C153" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D153" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F153" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I153">
         <v>1</v>
@@ -6775,16 +6775,16 @@
         <v>170</v>
       </c>
       <c r="B154" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C154" t="s">
+        <v>453</v>
+      </c>
+      <c r="D154" t="s">
         <v>454</v>
       </c>
-      <c r="D154" t="s">
-        <v>455</v>
-      </c>
       <c r="F154" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I154">
         <v>1000000000</v>
@@ -6798,19 +6798,19 @@
         <v>160</v>
       </c>
       <c r="B155" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C155" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D155" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E155" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F155" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I155">
         <v>1000</v>
@@ -6824,16 +6824,16 @@
         <v>230</v>
       </c>
       <c r="B156" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C156" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D156" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F156" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I156">
         <v>1000000000</v>
@@ -6847,16 +6847,16 @@
         <v>228</v>
       </c>
       <c r="B157" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C157" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D157" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F157" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I157">
         <v>1000000000</v>
@@ -6870,16 +6870,16 @@
         <v>158</v>
       </c>
       <c r="B158" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C158" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D158" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F158" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I158">
         <v>1</v>
@@ -6893,16 +6893,16 @@
         <v>162</v>
       </c>
       <c r="B159" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C159" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D159" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F159" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I159">
         <v>1</v>
@@ -6916,16 +6916,16 @@
         <v>164</v>
       </c>
       <c r="B160" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C160" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D160" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F160" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I160">
         <v>1</v>
@@ -6939,16 +6939,16 @@
         <v>293</v>
       </c>
       <c r="B161" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C161" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D161" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F161" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I161">
         <v>1</v>
@@ -6962,16 +6962,16 @@
         <v>168</v>
       </c>
       <c r="B162" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C162" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D162" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F162" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I162">
         <v>1</v>
@@ -6985,16 +6985,16 @@
         <v>265</v>
       </c>
       <c r="B163" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C163" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D163" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F163" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I163">
         <v>1E-3</v>
@@ -7008,19 +7008,19 @@
         <v>208</v>
       </c>
       <c r="B164" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C164" t="s">
+        <v>477</v>
+      </c>
+      <c r="D164" t="s">
         <v>478</v>
       </c>
-      <c r="D164" t="s">
-        <v>479</v>
-      </c>
       <c r="E164" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F164" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I164" s="1">
         <v>1.0000000000000001E-15</v>
@@ -7034,25 +7034,25 @@
         <v>152</v>
       </c>
       <c r="B165" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C165" t="s">
+        <v>441</v>
+      </c>
+      <c r="D165" t="s">
         <v>442</v>
       </c>
-      <c r="D165" t="s">
-        <v>443</v>
-      </c>
       <c r="E165" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F165" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G165" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H165" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I165" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7066,25 +7066,25 @@
         <v>150</v>
       </c>
       <c r="B166" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C166" t="s">
+        <v>439</v>
+      </c>
+      <c r="D166" t="s">
         <v>440</v>
       </c>
-      <c r="D166" t="s">
-        <v>441</v>
-      </c>
       <c r="E166" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F166" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G166" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H166" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I166" s="1">
         <v>1.0000000000000001E-15</v>
@@ -7098,19 +7098,19 @@
         <v>154</v>
       </c>
       <c r="B167" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C167" t="s">
+        <v>443</v>
+      </c>
+      <c r="D167" t="s">
         <v>444</v>
       </c>
-      <c r="D167" t="s">
-        <v>445</v>
-      </c>
       <c r="E167" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F167" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I167" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7124,19 +7124,19 @@
         <v>32</v>
       </c>
       <c r="B168" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C168" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D168" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E168" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F168" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I168" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7150,19 +7150,19 @@
         <v>283</v>
       </c>
       <c r="B169" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C169" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D169" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E169" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F169" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I169" s="1">
         <v>1.0000000000000001E-9</v>
@@ -7176,16 +7176,16 @@
         <v>156</v>
       </c>
       <c r="B170" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C170" t="s">
+        <v>445</v>
+      </c>
+      <c r="D170" t="s">
         <v>446</v>
       </c>
-      <c r="D170" t="s">
-        <v>447</v>
-      </c>
       <c r="F170" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I170" s="1">
         <v>1.1574074074074101E-14</v>
@@ -7199,16 +7199,16 @@
         <v>281</v>
       </c>
       <c r="B171" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C171" t="s">
+        <v>521</v>
+      </c>
+      <c r="D171" t="s">
         <v>522</v>
       </c>
-      <c r="D171" t="s">
-        <v>523</v>
-      </c>
       <c r="F171" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I171" s="1">
         <v>2.77777777777778E-13</v>
@@ -7222,16 +7222,16 @@
         <v>279</v>
       </c>
       <c r="B172" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C172" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D172" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F172" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I172" s="1">
         <v>1.15740740740741E-17</v>
@@ -7245,19 +7245,19 @@
         <v>277</v>
       </c>
       <c r="B173" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C173" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D173" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E173" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F173" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I173" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7271,16 +7271,16 @@
         <v>297</v>
       </c>
       <c r="B174" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C174" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D174" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F174" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I174" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7294,16 +7294,16 @@
         <v>299</v>
       </c>
       <c r="B175" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C175" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D175" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F175" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I175" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7317,16 +7317,16 @@
         <v>172</v>
       </c>
       <c r="B176" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C176" t="s">
+        <v>455</v>
+      </c>
+      <c r="D176" t="s">
         <v>456</v>
       </c>
-      <c r="D176" t="s">
-        <v>457</v>
-      </c>
       <c r="F176" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I176">
         <v>1.0000000000000001E-5</v>
@@ -7340,16 +7340,16 @@
         <v>295</v>
       </c>
       <c r="B177" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C177" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D177" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F177" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I177" s="1">
         <v>2.7777777777777802E-7</v>
@@ -7360,19 +7360,19 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B178" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C178" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D178" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F178" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I178" s="1">
         <v>9.9999999999999998E-13</v>
@@ -7386,16 +7386,16 @@
         <v>174</v>
       </c>
       <c r="B179" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C179" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D179" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F179" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I179">
         <v>1</v>
@@ -7409,16 +7409,16 @@
         <v>325</v>
       </c>
       <c r="B180" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C180" t="s">
+        <v>544</v>
+      </c>
+      <c r="D180" t="s">
         <v>545</v>
       </c>
-      <c r="D180" t="s">
-        <v>546</v>
-      </c>
       <c r="F180" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I180">
         <v>1</v>
@@ -7432,16 +7432,16 @@
         <v>319</v>
       </c>
       <c r="B181" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C181" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D181" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F181" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I181">
         <v>1</v>
@@ -7455,16 +7455,16 @@
         <v>321</v>
       </c>
       <c r="B182" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C182" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D182" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F182" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I182">
         <v>1</v>
@@ -7478,16 +7478,16 @@
         <v>323</v>
       </c>
       <c r="B183" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C183" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D183" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F183" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I183">
         <v>1</v>
@@ -7501,16 +7501,16 @@
         <v>315</v>
       </c>
       <c r="B184" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C184" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D184" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F184" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I184">
         <v>1000000000</v>
@@ -7524,16 +7524,16 @@
         <v>317</v>
       </c>
       <c r="B185" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C185" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D185" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F185" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I185">
         <v>1000000000</v>
@@ -7547,19 +7547,19 @@
         <v>327</v>
       </c>
       <c r="B186" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C186" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D186" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E186" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F186" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I186">
         <v>1</v>

</xml_diff>